<commit_message>
Site changes for JETT 0.8.0.
</commit_message>
<xml_diff>
--- a/jett-core/templates/NameTagTemplate.xlsx
+++ b/jett-core/templates/NameTagTemplate.xlsx
@@ -354,11 +354,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94513024"/>
-        <c:axId val="94514560"/>
+        <c:axId val="60034432"/>
+        <c:axId val="73299072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94513024"/>
+        <c:axId val="60034432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -367,7 +367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94514560"/>
+        <c:crossAx val="73299072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -376,7 +376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94514560"/>
+        <c:axId val="73299072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,7 +387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94513024"/>
+        <c:crossAx val="60034432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -503,11 +503,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="95931392"/>
-        <c:axId val="95936512"/>
+        <c:axId val="73488256"/>
+        <c:axId val="73489792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95931392"/>
+        <c:axId val="73488256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,7 +516,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95936512"/>
+        <c:crossAx val="73489792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -524,7 +524,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95936512"/>
+        <c:axId val="73489792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95931392"/>
+        <c:crossAx val="73488256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -596,15 +596,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1276350</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">

</xml_diff>